<commit_message>
made data dumping dynamic
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="48">
   <si>
     <t>TimeStamp</t>
   </si>
   <si>
-    <t>2023/07/02 23:32:59</t>
+    <t>2023/07/04 23:41:27</t>
   </si>
   <si>
     <t>Companies Name</t>
@@ -29,25 +29,29 @@
     <t>Current Price</t>
   </si>
   <si>
-    <t>2,550.25</t>
+    <t>—</t>
   </si>
   <si>
     <t>1d</t>
   </si>
   <si>
     <t>High
-₹ 2,556.65</t>
+₹ 2,625.00</t>
   </si>
   <si>
     <t>Low
-₹ 2,533.45</t>
-  </si>
-  <si>
-    <t>Returns
-0.82%</t>
+₹ 2,573.25</t>
+  </si>
+  <si>
+    <t>Returns
+1.03%</t>
   </si>
   <si>
     <t>1w</t>
+  </si>
+  <si>
+    <t>High
+₹ 2,622.00</t>
   </si>
   <si>
     <t>Low
@@ -55,22 +59,18 @@
   </si>
   <si>
     <t>Returns
-1.73%</t>
+4.77%</t>
   </si>
   <si>
     <t>1mo</t>
   </si>
   <si>
-    <t>High
-₹ 2,584.00</t>
-  </si>
-  <si>
     <t>Low
-₹ 2,451.00</t>
-  </si>
-  <si>
-    <t>Returns
-3.21%</t>
+₹ 2,458.45</t>
+  </si>
+  <si>
+    <t>Returns
+6.02%</t>
   </si>
   <si>
     <t>1y</t>
@@ -85,7 +85,7 @@
   </si>
   <si>
     <t>Returns
-5.66%</t>
+7.25%</t>
   </si>
   <si>
     <t>5y</t>
@@ -100,7 +100,7 @@
   </si>
   <si>
     <t>Returns
-165.49%</t>
+161.46%</t>
   </si>
   <si>
     <t>max</t>
@@ -111,7 +111,7 @@
   </si>
   <si>
     <t>Returns
-5,163.67%</t>
+5,243.14%</t>
   </si>
   <si>
     <t>sip</t>
@@ -122,11 +122,11 @@
   </si>
   <si>
     <t>Value
-₹ 8,597.24</t>
-  </si>
-  <si>
-    <t>Returns
-43.29%</t>
+₹ 8,610.26</t>
+  </si>
+  <si>
+    <t>Returns
+43.50%</t>
   </si>
   <si>
     <t>Performance</t>
@@ -159,95 +159,22 @@
     <t>PB Ratio</t>
   </si>
   <si>
-    <t>1.93</t>
+    <t>1.99</t>
   </si>
   <si>
     <t>Dividend Yeild</t>
   </si>
   <si>
-    <t>—</t>
-  </si>
-  <si>
-    <t>2023/07/02 23:33:35</t>
+    <t>2023/07/04 23:41:55</t>
   </si>
   <si>
     <t>TATAMOTORS</t>
   </si>
   <si>
-    <t>595.55</t>
-  </si>
-  <si>
-    <t>High
-₹ 599.00</t>
-  </si>
-  <si>
-    <t>Low
-₹ 588.00</t>
-  </si>
-  <si>
-    <t>Returns
-1.52%</t>
-  </si>
-  <si>
-    <t>Low
-₹ 557.80</t>
-  </si>
-  <si>
-    <t>Returns
-6.35%</t>
-  </si>
-  <si>
-    <t>Low
-₹ 532.75</t>
-  </si>
-  <si>
-    <t>Returns
-10.85%</t>
-  </si>
-  <si>
-    <t>Low
-₹ 375.20</t>
-  </si>
-  <si>
-    <t>Returns
-45.81%</t>
-  </si>
-  <si>
-    <t>Low
-₹ 63.50</t>
-  </si>
-  <si>
-    <t>Returns
-123.30%</t>
-  </si>
-  <si>
-    <t>High
-₹ 612.40</t>
-  </si>
-  <si>
-    <t>Low
-₹ 11.50</t>
-  </si>
-  <si>
-    <t>Returns
-1,273.82%</t>
-  </si>
-  <si>
-    <t>Value
-₹ 16,744.13</t>
-  </si>
-  <si>
-    <t>Returns
-179.07%</t>
+    <t/>
   </si>
   <si>
     <t>Good</t>
-  </si>
-  <si>
-    <t>4.01</t>
-  </si>
-  <si>
-    <t>0.32%</t>
   </si>
 </sst>
 </file>
@@ -292,7 +219,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -315,7 +242,7 @@
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
         <v>17</v>
@@ -368,10 +295,10 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
         <v>18</v>
@@ -407,7 +334,7 @@
         <v>42</v>
       </c>
       <c r="R2" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -415,7 +342,7 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
@@ -438,7 +365,7 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
         <v>16</v>
@@ -456,162 +383,162 @@
         <v>31</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" t="s">
+        <v>39</v>
+      </c>
+      <c r="P5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>46</v>
+      </c>
+      <c r="R5" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="I6" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="J6" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="K6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="O6" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="P6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="Q6" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="R6" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" t="s">
-        <v>47</v>
-      </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I7" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="J7" t="s">
-        <v>29</v>
-      </c>
-      <c r="K7" t="s">
-        <v>33</v>
-      </c>
-      <c r="L7" t="s">
-        <v>35</v>
-      </c>
-      <c r="M7" t="s">
-        <v>37</v>
-      </c>
-      <c r="N7" t="s">
-        <v>35</v>
-      </c>
-      <c r="O7" t="s">
-        <v>64</v>
-      </c>
-      <c r="P7" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>65</v>
-      </c>
-      <c r="R7" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8">
       <c r="D8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F8" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G8" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="H8" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="I8" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="J8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="D9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" t="s">
-        <v>58</v>
-      </c>
-      <c r="I9" t="s">
-        <v>61</v>
-      </c>
-      <c r="J9" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>